<commit_message>
Added New test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/dataSheet/NidaanTestData.xlsx
+++ b/src/test/resources/dataSheet/NidaanTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aditi.balur\Downloads\bk_automation_testng_prototype-master\bk_automation_testng_prototype-master\bk_automation_testNG_prototype\src\test\resources\dataSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aditi\EclipseWorkspace\DemoPipeline\DemoPipeline\src\test\resources\dataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD4FC7-F5B0-4900-A1CE-7932EA1F04FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D42C0FA-0FEC-413C-B395-787764E01593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{1E70CCEB-B519-2340-A0D6-827872CDD493}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{1E70CCEB-B519-2340-A0D6-827872CDD493}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="LoginData" sheetId="3" r:id="rId4"/>
     <sheet name="InvalidLoginData" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Test Steps</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>800377</t>
+  </si>
+  <si>
+    <t>9461247879</t>
+  </si>
+  <si>
+    <t>737373</t>
+  </si>
+  <si>
+    <t>9351111196</t>
+  </si>
+  <si>
+    <t>935196</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -224,6 +236,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F7A17C-97B6-469A-B2D9-43ABFABC23D6}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -743,10 +756,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AD0CFE-F178-DB43-95FD-EA2A075B2340}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -775,6 +788,28 @@
       </c>
       <c r="C2" s="4" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>